<commit_message>
Validate them 1 it employeeManagement
</commit_message>
<xml_diff>
--- a/src/testdata/clientDta.xlsx
+++ b/src/testdata/clientDta.xlsx
@@ -3837,8 +3837,8 @@
   <sheetPr/>
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="61" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="4"/>

</xml_diff>